<commit_message>
Update electricity and supply sectors
</commit_message>
<xml_diff>
--- a/BY_Trans.xlsx
+++ b/BY_Trans.xlsx
@@ -1,43 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VEDA_Models\Irish-TIMES_v2\Irish-TIMES_2p0_v03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_5E61D69B88F4659C736276255A921FE81B5B8486" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="870" windowWidth="16905" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="870" windowWidth="16905" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="Trans Tables" sheetId="17" r:id="rId1"/>
     <sheet name="FILL Table" sheetId="19" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Maurizio Gargiulo</author>
     <author>Gary Goldstein</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="H5" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M5" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="M5" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H13" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="H13" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -104,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M13" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="M13" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,77 +113,77 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
+    <t>~TFM_INS</t>
+  </si>
+  <si>
+    <t>~TFM_UPD</t>
+  </si>
+  <si>
+    <t>TimeSlice</t>
+  </si>
+  <si>
+    <t>LimType</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Pset_Set</t>
+  </si>
+  <si>
+    <t>Pset_PN</t>
+  </si>
+  <si>
+    <t>Pset_CI</t>
+  </si>
+  <si>
+    <t>Pset_CO</t>
+  </si>
+  <si>
+    <t>Cset_Set</t>
+  </si>
+  <si>
+    <t>Cset_CN</t>
+  </si>
+  <si>
+    <t>Cset_CD</t>
+  </si>
+  <si>
+    <t>Pset_PD</t>
+  </si>
+  <si>
     <t>* Parameter values for qualifying technologies in each region, not tied to BASE</t>
   </si>
   <si>
-    <t>~TFM_UPD</t>
-  </si>
-  <si>
-    <t>TimeSlice</t>
-  </si>
-  <si>
-    <t>LimType</t>
-  </si>
-  <si>
-    <t>Attribute</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t>AllRegions</t>
   </si>
   <si>
+    <t>~TFM_FILL</t>
+  </si>
+  <si>
+    <t>Operation_Sum_Avg_Count</t>
+  </si>
+  <si>
+    <t>Scenario Name</t>
+  </si>
+  <si>
+    <t>Other_Indexes</t>
+  </si>
+  <si>
+    <t>Tech_Comm_Info</t>
+  </si>
+  <si>
     <t>IE</t>
-  </si>
-  <si>
-    <t>Pset_Set</t>
-  </si>
-  <si>
-    <t>Pset_PN</t>
-  </si>
-  <si>
-    <t>Pset_PD</t>
-  </si>
-  <si>
-    <t>Pset_CI</t>
-  </si>
-  <si>
-    <t>Pset_CO</t>
-  </si>
-  <si>
-    <t>Cset_Set</t>
-  </si>
-  <si>
-    <t>Cset_CN</t>
-  </si>
-  <si>
-    <t>Cset_CD</t>
-  </si>
-  <si>
-    <t>~TFM_INS</t>
-  </si>
-  <si>
-    <t>~TFM_FILL</t>
-  </si>
-  <si>
-    <t>Operation_Sum_Avg_Count</t>
-  </si>
-  <si>
-    <t>Scenario Name</t>
-  </si>
-  <si>
-    <t>Other_Indexes</t>
-  </si>
-  <si>
-    <t>Tech_Comm_Info</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -203,6 +192,12 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -239,6 +234,12 @@
       <b/>
       <sz val="10"/>
       <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -305,22 +306,22 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,13 +659,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="5" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" style="5" customWidth="1"/>
@@ -687,136 +688,136 @@
     <col min="23" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:15" ht="15">
+    <row r="3" spans="2:15" ht="15" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
     </row>
-    <row r="6" spans="2:15" ht="22.5" customHeight="1" thickBot="1">
-      <c r="B6" s="11" t="s">
+    <row r="6" spans="2:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="I6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="J6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="L6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="M6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="N6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="O6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="7" t="s">
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+    </row>
+    <row r="14" spans="2:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-    </row>
-    <row r="13" spans="2:15">
-      <c r="B13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-    </row>
-    <row r="14" spans="2:15" ht="21" customHeight="1" thickBot="1">
-      <c r="B14" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="7" t="s">
+      <c r="K14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="L14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="M14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="N14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L14" s="7" t="s">
+      <c r="O14" s="11" t="s">
         <v>12</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O14" s="7" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -829,12 +830,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
@@ -851,17 +852,17 @@
     <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="2:13">
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
@@ -876,22 +877,22 @@
         <v>5</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="L3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -900,18 +901,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e65a81a2b168daca9e55ef64af43d0c8">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04e5c3f63ef199a395775dc61bce0287" ns2:_="">
-    <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F4935B8855D2CD4A84AB51A7B8A3B83B" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6046aa80c6137ea7cd300941e6de6139">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="795b6ce3-4d29-4fa5-96ed-ea1b36830f13" xmlns:ns3="424ab569-3a9e-4e02-994b-fd1ed8ea43ac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8866ff8f472ea66287faba2f38092fc5" ns2:_="" ns3:_="">
+    <xsd:import namespace="795b6ce3-4d29-4fa5-96ed-ea1b36830f13"/>
+    <xsd:import namespace="424ab569-3a9e-4e02-994b-fd1ed8ea43ac"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -922,11 +915,8 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -934,7 +924,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3a32fc56-8470-4d77-ad86-bef2a7229878" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="795b6ce3-4d29-4fa5-96ed-ea1b36830f13" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -959,31 +949,34 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="12" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="424ab569-3a9e-4e02-994b-fd1ed8ea43ac" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="13" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1086,6 +1079,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1093,13 +1095,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42508B13-06D6-4F81-9977-988936623257}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4DD51E5-E7FA-461E-86EE-EDC7BE80D911}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB8563E2-8A23-4165-A2C1-F4DF01145BC3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEC2C90E-7347-4633-BAEC-4C03C7C9F8A9}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F223C6B7-A84E-4F23-A01F-B9FD0B4F2C1E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51BB782A-18EB-4EBF-A498-B297B424B3AF}"/>
 </file>
</xml_diff>

<commit_message>
Update cover in the remaining VT files
</commit_message>
<xml_diff>
--- a/BY_Trans.xlsx
+++ b/BY_Trans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC39C18B-ADEF-4650-9F73-9354BBA26270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF365F87-9043-419E-B86B-12BA5428FEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,6 @@
     <sheet name="Trans Tables" sheetId="17" r:id="rId2"/>
     <sheet name="FILL Table" sheetId="19" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
     <definedName name="_AtRisk_SimSetting_AutomaticallyGenerateReports" hidden="1">FALSE</definedName>
@@ -182,7 +179,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -256,25 +253,13 @@
     <t>Document type:</t>
   </si>
   <si>
-    <t>Template type</t>
-  </si>
-  <si>
     <t>Sector(s):</t>
-  </si>
-  <si>
-    <t>Sector name</t>
   </si>
   <si>
     <t>Purpose:</t>
   </si>
   <si>
-    <t>Brief description of what this file is for</t>
-  </si>
-  <si>
     <t>Original developer(s):</t>
-  </si>
-  <si>
-    <t>Full Name(s) (Affiliation, email)</t>
   </si>
   <si>
     <t>Current maintainer(s):</t>
@@ -296,6 +281,21 @@
   </si>
   <si>
     <t>https://creativecommons.org/licenses/by-nc-sa/4.0/</t>
+  </si>
+  <si>
+    <t>Base Year Transformation</t>
+  </si>
+  <si>
+    <t>All sectors</t>
+  </si>
+  <si>
+    <t>Specify region dependent base year data transformation</t>
+  </si>
+  <si>
+    <t>Automatically generated by Veda</t>
+  </si>
+  <si>
+    <t>Olexandr Balyk (UCC, olexandr.balyk@ucc.ie)</t>
   </si>
 </sst>
 </file>
@@ -537,9 +537,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -558,9 +555,6 @@
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -573,14 +567,20 @@
     <xf numFmtId="164" fontId="16" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -914,19 +914,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1251,8 +1238,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,20 +1677,20 @@
       <c r="Z15" s="14"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
       <c r="M16" s="14"/>
       <c r="N16" s="14"/>
       <c r="O16" s="14"/>
@@ -1720,10 +1707,10 @@
       <c r="Z16" s="14"/>
     </row>
     <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
@@ -1748,18 +1735,18 @@
       <c r="Z17" s="14"/>
     </row>
     <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
       <c r="M18" s="14"/>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
@@ -1776,22 +1763,22 @@
       <c r="Z18" s="14"/>
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
+      <c r="B19" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
       <c r="M19" s="14"/>
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
@@ -1808,22 +1795,22 @@
       <c r="Z19" s="14"/>
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
+      <c r="A20" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
       <c r="M20" s="14"/>
       <c r="N20" s="14"/>
       <c r="O20" s="14"/>
@@ -1840,22 +1827,22 @@
       <c r="Z20" s="14"/>
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
+      <c r="A21" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
       <c r="M21" s="14"/>
       <c r="N21" s="14"/>
       <c r="O21" s="14"/>
@@ -1872,18 +1859,18 @@
       <c r="Z21" s="14"/>
     </row>
     <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
       <c r="M22" s="14"/>
       <c r="N22" s="14"/>
       <c r="O22" s="14"/>
@@ -1900,14 +1887,14 @@
       <c r="Z22" s="14"/>
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
+      <c r="A23" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
@@ -1932,10 +1919,10 @@
       <c r="Z23" s="14"/>
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -1960,10 +1947,10 @@
       <c r="Z24" s="14"/>
     </row>
     <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
@@ -1988,14 +1975,14 @@
       <c r="Z25" s="14"/>
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
+      <c r="A26" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -2020,10 +2007,10 @@
       <c r="Z26" s="14"/>
     </row>
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -2048,10 +2035,10 @@
       <c r="Z27" s="14"/>
     </row>
     <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
@@ -2076,14 +2063,14 @@
       <c r="Z28" s="14"/>
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="27">
+      <c r="A29" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="25">
         <v>1</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
@@ -2108,16 +2095,16 @@
       <c r="Z29" s="14"/>
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
+      <c r="A30" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
@@ -2140,16 +2127,16 @@
       <c r="Z30" s="14"/>
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
+      <c r="A31" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
@@ -2172,12 +2159,12 @@
       <c r="Z31" s="14"/>
     </row>
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
@@ -4341,21 +4328,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F4935B8855D2CD4A84AB51A7B8A3B83B" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6046aa80c6137ea7cd300941e6de6139">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="795b6ce3-4d29-4fa5-96ed-ea1b36830f13" xmlns:ns3="424ab569-3a9e-4e02-994b-fd1ed8ea43ac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8866ff8f472ea66287faba2f38092fc5" ns2:_="" ns3:_="">
     <xsd:import namespace="795b6ce3-4d29-4fa5-96ed-ea1b36830f13"/>
@@ -4534,24 +4506,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51BB782A-18EB-4EBF-A498-B297B424B3AF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEC2C90E-7347-4633-BAEC-4C03C7C9F8A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4DD51E5-E7FA-461E-86EE-EDC7BE80D911}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4568,4 +4538,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEC2C90E-7347-4633-BAEC-4C03C7C9F8A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51BB782A-18EB-4EBF-A498-B297B424B3AF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>